<commit_message>
Fix off-by-one in eStInterRes for h0168
Implement possible fix for constraint-names in Pyomo-exported MPS files
Improve output of compareMPS
Add timing information for GAMS execution
Set RoR units to 0 (in Excel)
Disable investment in Storage (in Excel)
</commit_message>
<xml_diff>
--- a/data/example/Power_RoR.xlsx
+++ b/data/example/Power_RoR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix Auer\Local\Code\LEGO_internal\examples\001_Base_Example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5869DE2-DAB9-4DBF-9913-454C19310B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64999A0-0450-4D1B-986A-49834B321A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-17544" windowWidth="30936" windowHeight="16776" xr2:uid="{781DDF88-8197-4A3B-8B6A-9D54FE0618CA}"/>
+    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{781DDF88-8197-4A3B-8B6A-9D54FE0618CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Power RoR" sheetId="2" r:id="rId1"/>
@@ -927,53 +927,53 @@
       <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.36328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.1796875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.140625" style="7" customWidth="1"/>
     <col min="5" max="5" width="13" style="7" customWidth="1"/>
     <col min="6" max="6" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.36328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.36328125" style="7" customWidth="1"/>
-    <col min="29" max="30" width="10.81640625" style="7" customWidth="1"/>
-    <col min="31" max="32" width="8.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.36328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="10.36328125" style="7"/>
+    <col min="21" max="21" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.42578125" style="7" customWidth="1"/>
+    <col min="29" max="30" width="10.85546875" style="7" customWidth="1"/>
+    <col min="31" max="32" width="8.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="10.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1002,7 +1002,7 @@
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>45</v>
       </c>
@@ -1098,7 +1098,7 @@
       <c r="AI3" s="10"/>
       <c r="AJ3" s="10"/>
     </row>
-    <row r="4" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="13"/>
@@ -1133,7 +1133,7 @@
       <c r="AI4" s="10"/>
       <c r="AJ4" s="10"/>
     </row>
-    <row r="5" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22"/>
       <c r="E5" s="14"/>
       <c r="F5" s="13"/>
@@ -1168,7 +1168,7 @@
       <c r="AI5" s="10"/>
       <c r="AJ5" s="10"/>
     </row>
-    <row r="6" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="E6" s="15" t="s">
         <v>6</v>
@@ -1245,7 +1245,7 @@
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>36</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="16">
         <v>25.4</v>
@@ -1322,7 +1322,7 @@
         <v>14.4793</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="G9" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Szenarios for comparison Link
</commit_message>
<xml_diff>
--- a/data/example/Power_RoR.xlsx
+++ b/data/example/Power_RoR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suess\Desktop\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64999A0-0450-4D1B-986A-49834B321A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A125BF48-3995-462F-BF2F-5111C3F3E093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{781DDF88-8197-4A3B-8B6A-9D54FE0618CA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{781DDF88-8197-4A3B-8B6A-9D54FE0618CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Power RoR" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <definedName name="param">#REF!</definedName>
     <definedName name="renewable">#REF!</definedName>
     <definedName name="resprofile">#REF!</definedName>
-    <definedName name="runofriver">'Power RoR'!$B$2:$AB$7</definedName>
+    <definedName name="runofriver">'Power RoR'!$B$2:$AB$6</definedName>
     <definedName name="sCodeName">#REF!</definedName>
     <definedName name="thermalgen">#REF!</definedName>
     <definedName name="weight_k">#REF!</definedName>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -320,15 +320,6 @@
     <t>Power - Run of River</t>
   </si>
   <si>
-    <t>RoR1</t>
-  </si>
-  <si>
-    <t>RoR</t>
-  </si>
-  <si>
-    <t>Node_1</t>
-  </si>
-  <si>
     <t>PPName</t>
   </si>
   <si>
@@ -342,9 +333,6 @@
   </si>
   <si>
     <t>long</t>
-  </si>
-  <si>
-    <t>RoR_Test1</t>
   </si>
   <si>
     <t>Excl.</t>
@@ -354,9 +342,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -464,7 +451,7 @@
       <name val="Aptos"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,12 +478,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -515,17 +496,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -556,14 +531,7 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -579,9 +547,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Data" xfId="3" xr:uid="{5F141EC6-8E4D-6640-9A98-4DC436FB450B}"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{932C65E5-CB5D-4C06-8800-B5B605222250}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -921,409 +889,332 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="A1:AJ9"/>
+  <dimension ref="A1:AJ8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="12.140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.42578125" style="7" customWidth="1"/>
-    <col min="29" max="30" width="10.85546875" style="7" customWidth="1"/>
-    <col min="31" max="32" width="8.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="10.42578125" style="7"/>
+    <col min="1" max="1" width="5.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.42578125" style="5" customWidth="1"/>
+    <col min="29" max="30" width="10.85546875" style="5" customWidth="1"/>
+    <col min="31" max="32" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="10.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:36" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
     </row>
-    <row r="3" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9" t="s">
+    <row r="3" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="O3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="S3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="T3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="U3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="V3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="W3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="X3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="Y3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Z3" s="9" t="s">
+      <c r="Z3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="9" t="s">
+      <c r="AA3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AB3" s="9" t="s">
+      <c r="AB3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" s="9" t="s">
+      <c r="AF3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AD3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
     </row>
-    <row r="4" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="13"/>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="13"/>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
+    <row r="4" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
     </row>
-    <row r="5" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="10"/>
-      <c r="AH5" s="10"/>
-      <c r="AI5" s="10"/>
-      <c r="AJ5" s="10"/>
+    <row r="5" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
     </row>
-    <row r="6" spans="1:36" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="E6" s="15" t="s">
+    <row r="6" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="E6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="15" t="s">
+      <c r="N6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="P6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="15" t="s">
+      <c r="Q6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="R6" s="15" t="s">
+      <c r="R6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="S6" s="15" t="s">
+      <c r="S6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="T6" s="15" t="s">
+      <c r="T6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="U6" s="15" t="s">
+      <c r="U6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="V6" s="15" t="s">
+      <c r="V6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="W6" s="15" t="s">
+      <c r="W6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="X6" s="15" t="s">
+      <c r="X6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="15" t="s">
+      <c r="Y6" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="8"/>
-      <c r="AH6" s="8"/>
-      <c r="AI6" s="8"/>
-      <c r="AJ6" s="8"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="19">
-        <v>0</v>
-      </c>
-      <c r="F7" s="16">
-        <v>25.4</v>
-      </c>
-      <c r="G7" s="16">
-        <v>0</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16">
-        <v>0.92</v>
-      </c>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16">
-        <v>12.7</v>
-      </c>
-      <c r="L7" s="16">
-        <v>-12.7</v>
-      </c>
-      <c r="M7" s="16">
-        <v>2</v>
-      </c>
-      <c r="N7" s="16">
-        <v>1</v>
-      </c>
-      <c r="O7" s="16">
-        <v>0</v>
-      </c>
-      <c r="P7" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="16">
-        <v>0</v>
-      </c>
-      <c r="R7" s="16">
-        <v>0</v>
-      </c>
-      <c r="S7" s="16">
-        <v>0</v>
-      </c>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16">
-        <v>0</v>
-      </c>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16">
-        <v>0.25</v>
-      </c>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="16"/>
-      <c r="AB7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC7" s="2">
-        <v>1981</v>
-      </c>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="3">
-        <v>46.561399999999999</v>
-      </c>
-      <c r="AF7" s="3">
-        <v>14.4793</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="G9" s="17"/>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="G8" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>